<commit_message>
Update on 20250819 part 8
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/webview频道统计.xlsx
+++ b/直播源汇总文档/其他文档/webview频道统计.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="657">
   <si>
     <t>北京卫视,webview://https://yangshipin.cn/tv/home?pid=600002309</t>
   </si>
@@ -811,9 +811,6 @@
     <t>南宁公共,webview://http://www.nntv.cn/live/nntv_gg/</t>
   </si>
   <si>
-    <t>柳州新闻综合,webview://https://web.guangdianyun.tv/tv/?id=1902&amp;uin=3370</t>
-  </si>
-  <si>
     <t>桂林新闻综合,webview://https://guilinbcnew.zainanjing365.com//share/live/detailTv?resourceId=33</t>
   </si>
   <si>
@@ -2032,6 +2029,22 @@
   </si>
   <si>
     <t>宁夏少儿,webview://https://web.ningxiahuangheyun.com/app/nxtv-tv/nxse/</t>
+  </si>
+  <si>
+    <t>柳州新闻综合,webview://https://web.guangdianyun.tv/tv/?id=1902&amp;uin=3370</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柳州科教,webview://https://live.lzgd.com.cn/tv/1808?uin=3370</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柳州新闻综合,webview://https://live.lzgd.com.cn/tv/1902?uin=3370</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柳州科教,webview://https://web.guangdianyun.tv/tv/?id=1808&amp;uin=3370</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2396,7 +2409,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
@@ -2740,47 +2753,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2802,27 +2815,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2841,87 +2854,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2943,162 +2956,162 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3122,52 +3135,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -3224,102 +3237,102 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3341,62 +3354,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3418,42 +3431,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3475,92 +3488,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3582,87 +3595,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -4021,37 +4034,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -4073,27 +4086,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -4115,47 +4128,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -4177,32 +4190,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -4224,77 +4237,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -4316,187 +4329,187 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -4520,52 +4533,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
@@ -4575,32 +4588,32 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -4622,12 +4635,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
@@ -4662,187 +4675,187 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -4871,7 +4884,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -4893,162 +4906,162 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -5129,37 +5142,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -5181,122 +5194,122 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -5318,37 +5331,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
@@ -5358,172 +5371,172 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -5845,12 +5858,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
@@ -6076,7 +6089,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6137,72 +6150,87 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>655</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>653</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>253</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>254</v>
+        <v>656</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>